<commit_message>
First version of caffeine network
</commit_message>
<xml_diff>
--- a/python/multiscalepy/multiscale/modelcreator/models/caffeine/caffeine_annotations.xlsx
+++ b/python/multiscalepy/multiscale/modelcreator/models/caffeine/caffeine_annotations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="262" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="439" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2192" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="348">
   <si>
     <t>pattern</t>
   </si>
@@ -707,7 +707,7 @@
     <t># species</t>
   </si>
   <si>
-    <t>^glc[_]*\w*$</t>
+    <t>^caf[_]*\w*$</t>
   </si>
   <si>
     <t>species</t>
@@ -719,22 +719,19 @@
     <t>simple chemical</t>
   </si>
   <si>
-    <t>CHEBI:4167</t>
-  </si>
-  <si>
-    <t>D-glucopyranose</t>
-  </si>
-  <si>
-    <t>C00031</t>
-  </si>
-  <si>
-    <t>D-Glucose</t>
+    <t>CHEBI:27732</t>
+  </si>
+  <si>
+    <t>caffeine</t>
+  </si>
+  <si>
+    <t>C07481</t>
   </si>
   <si>
     <t>Formula</t>
   </si>
   <si>
-    <t>C6H12O6</t>
+    <t>C8H10N4O2</t>
   </si>
   <si>
     <t>Charge</t>
@@ -743,6 +740,56 @@
     <t>0</t>
   </si>
   <si>
+    <t>^px[_]*\w*$</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CHEBI:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">25858</t>
+    </r>
+  </si>
+  <si>
+    <t>1,7-dimethylxanthine</t>
+  </si>
+  <si>
+    <t>C13747</t>
+  </si>
+  <si>
+    <t>C7H8N4O2</t>
+  </si>
+  <si>
+    <t>^tb[_]*\w*$</t>
+  </si>
+  <si>
+    <t>CHEBI:28946</t>
+  </si>
+  <si>
+    <t>theobromine</t>
+  </si>
+  <si>
+    <t>C07480</t>
+  </si>
+  <si>
+    <t>^tp[_]*\w*$</t>
+  </si>
+  <si>
+    <t>CHEBI:28177</t>
+  </si>
+  <si>
+    <t>theophylline</t>
+  </si>
+  <si>
+    <t>C07130</t>
+  </si>
+  <si>
     <t>^atp[_]*\w*$</t>
   </si>
   <si>
@@ -1008,279 +1055,6 @@
   </si>
   <si>
     <t>H2O</t>
-  </si>
-  <si>
-    <t>^glc1p[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00103</t>
-  </si>
-  <si>
-    <t>D-Glucose 1-phosphate</t>
-  </si>
-  <si>
-    <t>CHEBI:58601</t>
-  </si>
-  <si>
-    <t>alpha-D-glucose 1-phosphate(2-)</t>
-  </si>
-  <si>
-    <t>C6H11O9P</t>
-  </si>
-  <si>
-    <t>^udpglc[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00029</t>
-  </si>
-  <si>
-    <t>UDP-glucose</t>
-  </si>
-  <si>
-    <t>CHEBI:58885</t>
-  </si>
-  <si>
-    <t>UDP-alpha-D-glucose(2-)</t>
-  </si>
-  <si>
-    <t>C15H22N2O17P2</t>
-  </si>
-  <si>
-    <t>^glyglc[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00182</t>
-  </si>
-  <si>
-    <t>CHEBI:28087</t>
-  </si>
-  <si>
-    <t>^glc6p[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00668</t>
-  </si>
-  <si>
-    <t>alpha-D-Glucose 6-phosphate</t>
-  </si>
-  <si>
-    <t>CHEBI:61548</t>
-  </si>
-  <si>
-    <t>D-glucopyranose 6-phosphate(2-)</t>
-  </si>
-  <si>
-    <t>^fru6p[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00085</t>
-  </si>
-  <si>
-    <t>CHEBI:57579</t>
-  </si>
-  <si>
-    <t>D-fructose 6-phosphate(2−)</t>
-  </si>
-  <si>
-    <t>^fru16bp[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00354</t>
-  </si>
-  <si>
-    <t>CHEBI:49299</t>
-  </si>
-  <si>
-    <t>D-fructofuranose 1,6-bisphosphate(4-)</t>
-  </si>
-  <si>
-    <t>C6H10O12P2</t>
-  </si>
-  <si>
-    <t>^fru26bp[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00665</t>
-  </si>
-  <si>
-    <t>CHEBI:58579</t>
-  </si>
-  <si>
-    <t>β-D-fructofuranose 2,6-bisphosphate(4−)</t>
-  </si>
-  <si>
-    <t>^grap[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00118</t>
-  </si>
-  <si>
-    <t>CHEBI:59776</t>
-  </si>
-  <si>
-    <t>D-glyceraldehyde 3-phosphate(2-)</t>
-  </si>
-  <si>
-    <t>C3H5O6P</t>
-  </si>
-  <si>
-    <t>^dhap[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00111</t>
-  </si>
-  <si>
-    <t>CHEBI:57642</t>
-  </si>
-  <si>
-    <t>glycerone phosphate(2-)</t>
-  </si>
-  <si>
-    <t>^bpg13[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00236</t>
-  </si>
-  <si>
-    <t>CHEBI:57604</t>
-  </si>
-  <si>
-    <t>3-phosphonato-D-glyceroyl phosphate(4-)</t>
-  </si>
-  <si>
-    <t>C3H4O10P2</t>
-  </si>
-  <si>
-    <t>^pg3[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00197</t>
-  </si>
-  <si>
-    <t>CHEBI:58272</t>
-  </si>
-  <si>
-    <t>3-phosphonato-D-glycerate(3-)</t>
-  </si>
-  <si>
-    <t>C3H4O7P</t>
-  </si>
-  <si>
-    <t>^pg2[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00631</t>
-  </si>
-  <si>
-    <t>CHEBI:58289</t>
-  </si>
-  <si>
-    <t>2-phosphonato-D-glycerate(3-)</t>
-  </si>
-  <si>
-    <t>^pep[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00074</t>
-  </si>
-  <si>
-    <t>CHEBI:58702</t>
-  </si>
-  <si>
-    <t>phosphonatoenolpyruvate</t>
-  </si>
-  <si>
-    <t>C3H2O6P</t>
-  </si>
-  <si>
-    <t>^pyr[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00022</t>
-  </si>
-  <si>
-    <t>CHEBI:15361</t>
-  </si>
-  <si>
-    <t>pyruvate</t>
-  </si>
-  <si>
-    <t>C3H3O3</t>
-  </si>
-  <si>
-    <t>^oaa[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00036</t>
-  </si>
-  <si>
-    <t>CHEBI:16452</t>
-  </si>
-  <si>
-    <t>oxaloacetate(2-)</t>
-  </si>
-  <si>
-    <t>C4H2O5</t>
-  </si>
-  <si>
-    <t>^lac[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00186</t>
-  </si>
-  <si>
-    <t>CHEBI:16651</t>
-  </si>
-  <si>
-    <t>(S)-lactate</t>
-  </si>
-  <si>
-    <t>C3H5O3</t>
-  </si>
-  <si>
-    <t>^coa[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00010</t>
-  </si>
-  <si>
-    <t>CHEBI:57287</t>
-  </si>
-  <si>
-    <t>coenzyme A(4-)</t>
-  </si>
-  <si>
-    <t>C21H32N7O16P3S</t>
-  </si>
-  <si>
-    <t>^acoa[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00024</t>
-  </si>
-  <si>
-    <t>CHEBI:57288</t>
-  </si>
-  <si>
-    <t>acetyl-CoA(4-)</t>
-  </si>
-  <si>
-    <t>C23H34N7O17P3S</t>
-  </si>
-  <si>
-    <t>^cit[_]*\w*$</t>
-  </si>
-  <si>
-    <t>C00158</t>
-  </si>
-  <si>
-    <t>CHEBI:16947</t>
-  </si>
-  <si>
-    <t>citrate(3-)</t>
-  </si>
-  <si>
-    <t>C6H5O7</t>
   </si>
   <si>
     <t># rules</t>
@@ -1307,7 +1081,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1342,6 +1116,26 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00000A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00000A"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00000A"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1405,7 +1199,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1482,12 +1276,20 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1511,7 +1313,7 @@
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF00000A"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
@@ -1567,10 +1369,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G457"/>
+  <dimension ref="A1:G362"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A451" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B457" activeCellId="0" sqref="B457"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A226" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D266" activeCellId="0" sqref="D266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6259,7 +6061,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="7" t="s">
         <v>230</v>
       </c>
@@ -6269,7 +6071,7 @@
       <c r="C247" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D247" s="11" t="s">
+      <c r="D247" s="19" t="s">
         <v>234</v>
       </c>
       <c r="E247" s="7" t="s">
@@ -6278,7 +6080,7 @@
       <c r="F247" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G247" s="12" t="s">
+      <c r="G247" s="14" t="s">
         <v>235</v>
       </c>
     </row>
@@ -6292,7 +6094,7 @@
       <c r="C248" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D248" s="11" t="s">
+      <c r="D248" s="20" t="s">
         <v>236</v>
       </c>
       <c r="E248" s="7" t="s">
@@ -6302,7 +6104,7 @@
         <v>92</v>
       </c>
       <c r="G248" s="14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6313,10 +6115,10 @@
         <v>231</v>
       </c>
       <c r="C249" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D249" s="21" t="s">
         <v>238</v>
-      </c>
-      <c r="D249" s="7" t="s">
-        <v>239</v>
       </c>
       <c r="E249" s="7"/>
       <c r="F249" s="7"/>
@@ -6330,27 +6132,27 @@
         <v>231</v>
       </c>
       <c r="C250" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D250" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="D250" s="11" t="s">
-        <v>241</v>
       </c>
       <c r="E250" s="7"/>
       <c r="F250" s="7"/>
       <c r="G250" s="0"/>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="0"/>
-      <c r="B251" s="0"/>
-      <c r="C251" s="0"/>
-      <c r="D251" s="15"/>
-      <c r="E251" s="0"/>
-      <c r="F251" s="0"/>
+      <c r="A251" s="7"/>
+      <c r="B251" s="7"/>
+      <c r="C251" s="7"/>
+      <c r="D251" s="11"/>
+      <c r="E251" s="7"/>
+      <c r="F251" s="7"/>
       <c r="G251" s="0"/>
     </row>
     <row r="252" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="14" t="s">
-        <v>242</v>
+      <c r="A252" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="B252" s="7" t="s">
         <v>231</v>
@@ -6372,17 +6174,17 @@
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="14" t="s">
+      <c r="A253" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B253" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C253" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D253" s="19" t="s">
         <v>242</v>
-      </c>
-      <c r="B253" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C253" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D253" s="11" t="s">
-        <v>243</v>
       </c>
       <c r="E253" s="7" t="s">
         <v>22</v>
@@ -6391,78 +6193,78 @@
         <v>90</v>
       </c>
       <c r="G253" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B254" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C254" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D254" s="19" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="254" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="B254" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C254" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D254" s="11" t="s">
-        <v>245</v>
-      </c>
       <c r="E254" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F254" s="7" t="s">
         <v>92</v>
       </c>
       <c r="G254" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="255" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="14" t="s">
-        <v>242</v>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="B255" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C255" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D255" s="13" t="s">
-        <v>247</v>
+        <v>237</v>
+      </c>
+      <c r="D255" s="19" t="s">
+        <v>245</v>
       </c>
       <c r="E255" s="7"/>
       <c r="F255" s="7"/>
       <c r="G255" s="0"/>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="14" t="s">
-        <v>242</v>
+      <c r="A256" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="B256" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C256" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D256" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="D256" s="11" t="s">
-        <v>248</v>
       </c>
       <c r="E256" s="7"/>
       <c r="F256" s="7"/>
       <c r="G256" s="0"/>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="0"/>
+      <c r="A257" s="7"/>
       <c r="B257" s="7"/>
       <c r="C257" s="7"/>
-      <c r="D257" s="13"/>
+      <c r="D257" s="11"/>
       <c r="E257" s="7"/>
       <c r="F257" s="7"/>
       <c r="G257" s="0"/>
     </row>
     <row r="258" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="14" t="s">
-        <v>249</v>
+      <c r="A258" s="7" t="s">
+        <v>246</v>
       </c>
       <c r="B258" s="7" t="s">
         <v>231</v>
@@ -6484,8 +6286,8 @@
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="14" t="s">
-        <v>249</v>
+      <c r="A259" s="7" t="s">
+        <v>246</v>
       </c>
       <c r="B259" s="7" t="s">
         <v>231</v>
@@ -6493,8 +6295,8 @@
       <c r="C259" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D259" s="11" t="s">
-        <v>250</v>
+      <c r="D259" s="20" t="s">
+        <v>247</v>
       </c>
       <c r="E259" s="7" t="s">
         <v>22</v>
@@ -6503,78 +6305,78 @@
         <v>90</v>
       </c>
       <c r="G259" s="12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="14" t="s">
+      <c r="A260" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B260" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C260" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D260" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="B260" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C260" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D260" s="11" t="s">
-        <v>252</v>
-      </c>
       <c r="E260" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F260" s="7" t="s">
         <v>92</v>
       </c>
       <c r="G260" s="12" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="261" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="7" t="s">
+        <v>246</v>
       </c>
       <c r="B261" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C261" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D261" s="13" t="s">
-        <v>254</v>
+        <v>237</v>
+      </c>
+      <c r="D261" s="19" t="s">
+        <v>245</v>
       </c>
       <c r="E261" s="7"/>
       <c r="F261" s="7"/>
       <c r="G261" s="0"/>
     </row>
-    <row r="262" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="14" t="s">
-        <v>249</v>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="7" t="s">
+        <v>246</v>
       </c>
       <c r="B262" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C262" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D262" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="D262" s="13" t="n">
-        <v>-3</v>
       </c>
       <c r="E262" s="7"/>
       <c r="F262" s="7"/>
       <c r="G262" s="0"/>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="0"/>
+      <c r="A263" s="7"/>
       <c r="B263" s="7"/>
       <c r="C263" s="7"/>
-      <c r="D263" s="15"/>
+      <c r="D263" s="11"/>
       <c r="E263" s="7"/>
       <c r="F263" s="7"/>
       <c r="G263" s="0"/>
     </row>
     <row r="264" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="14" t="s">
-        <v>255</v>
+      <c r="A264" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="B264" s="7" t="s">
         <v>231</v>
@@ -6595,9 +6397,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="14" t="s">
-        <v>255</v>
+    <row r="265" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="B265" s="7" t="s">
         <v>231</v>
@@ -6605,8 +6407,8 @@
       <c r="C265" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D265" s="7" t="s">
-        <v>256</v>
+      <c r="D265" s="20" t="s">
+        <v>251</v>
       </c>
       <c r="E265" s="7" t="s">
         <v>22</v>
@@ -6614,13 +6416,13 @@
       <c r="F265" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G265" s="0" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="14" t="s">
-        <v>255</v>
+      <c r="G265" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="B266" s="7" t="s">
         <v>231</v>
@@ -6628,48 +6430,48 @@
       <c r="C266" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D266" s="7" t="s">
-        <v>258</v>
+      <c r="D266" s="20" t="s">
+        <v>253</v>
       </c>
       <c r="E266" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F266" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G266" s="0" t="s">
-        <v>259</v>
+      <c r="G266" s="12" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="14" t="s">
-        <v>255</v>
+      <c r="A267" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="B267" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C267" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D267" s="12" t="s">
-        <v>260</v>
+        <v>237</v>
+      </c>
+      <c r="D267" s="19" t="s">
+        <v>245</v>
       </c>
       <c r="E267" s="7"/>
       <c r="F267" s="7"/>
       <c r="G267" s="0"/>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="14" t="s">
-        <v>255</v>
+      <c r="A268" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="B268" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C268" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D268" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="D268" s="7" t="n">
-        <v>-2</v>
       </c>
       <c r="E268" s="7"/>
       <c r="F268" s="7"/>
@@ -6684,9 +6486,9 @@
       <c r="F269" s="0"/>
       <c r="G269" s="0"/>
     </row>
-    <row r="270" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="14" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B270" s="7" t="s">
         <v>231</v>
@@ -6707,9 +6509,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="14" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B271" s="7" t="s">
         <v>231</v>
@@ -6718,7 +6520,7 @@
         <v>11</v>
       </c>
       <c r="D271" s="11" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="E271" s="7" t="s">
         <v>22</v>
@@ -6727,12 +6529,12 @@
         <v>90</v>
       </c>
       <c r="G271" s="12" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="272" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="14" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B272" s="7" t="s">
         <v>231</v>
@@ -6741,7 +6543,7 @@
         <v>11</v>
       </c>
       <c r="D272" s="11" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E272" s="7" t="s">
         <v>33</v>
@@ -6750,21 +6552,21 @@
         <v>92</v>
       </c>
       <c r="G272" s="12" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="273" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="14" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B273" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C273" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D273" s="13" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E273" s="7"/>
       <c r="F273" s="7"/>
@@ -6772,33 +6574,33 @@
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="14" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B274" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C274" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D274" s="11" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="E274" s="7"/>
       <c r="F274" s="7"/>
       <c r="G274" s="0"/>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="14"/>
-      <c r="B275" s="0"/>
-      <c r="C275" s="0"/>
-      <c r="D275" s="15"/>
-      <c r="E275" s="0"/>
-      <c r="F275" s="0"/>
+      <c r="A275" s="0"/>
+      <c r="B275" s="7"/>
+      <c r="C275" s="7"/>
+      <c r="D275" s="13"/>
+      <c r="E275" s="7"/>
+      <c r="F275" s="7"/>
       <c r="G275" s="0"/>
     </row>
-    <row r="276" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="14" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B276" s="7" t="s">
         <v>231</v>
@@ -6819,9 +6621,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="14" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B277" s="7" t="s">
         <v>231</v>
@@ -6830,7 +6632,7 @@
         <v>11</v>
       </c>
       <c r="D277" s="11" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="E277" s="7" t="s">
         <v>22</v>
@@ -6839,12 +6641,12 @@
         <v>90</v>
       </c>
       <c r="G277" s="12" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="278" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="14" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B278" s="7" t="s">
         <v>231</v>
@@ -6853,7 +6655,7 @@
         <v>11</v>
       </c>
       <c r="D278" s="11" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="E278" s="7" t="s">
         <v>33</v>
@@ -6862,35 +6664,35 @@
         <v>92</v>
       </c>
       <c r="G278" s="12" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="279" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="14" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B279" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C279" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D279" s="13" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E279" s="7"/>
       <c r="F279" s="7"/>
       <c r="G279" s="0"/>
     </row>
-    <row r="280" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="14" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B280" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C280" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D280" s="13" t="n">
         <v>-3</v>
@@ -6901,16 +6703,16 @@
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0"/>
-      <c r="B281" s="0"/>
-      <c r="C281" s="0"/>
+      <c r="B281" s="7"/>
+      <c r="C281" s="7"/>
       <c r="D281" s="15"/>
-      <c r="E281" s="0"/>
-      <c r="F281" s="0"/>
+      <c r="E281" s="7"/>
+      <c r="F281" s="7"/>
       <c r="G281" s="0"/>
     </row>
-    <row r="282" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="14" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B282" s="7" t="s">
         <v>231</v>
@@ -6933,7 +6735,7 @@
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="14" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B283" s="7" t="s">
         <v>231</v>
@@ -6942,68 +6744,70 @@
         <v>11</v>
       </c>
       <c r="D283" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E283" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F283" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G283" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="B284" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C284" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D284" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E284" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F283" s="7" t="s">
+      <c r="F284" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G283" s="0"/>
-    </row>
-    <row r="284" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="B284" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C284" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D284" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="E284" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F284" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G284" s="19" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="285" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G284" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="14" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B285" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C285" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D285" s="13" t="s">
-        <v>277</v>
+        <v>237</v>
+      </c>
+      <c r="D285" s="12" t="s">
+        <v>272</v>
       </c>
       <c r="E285" s="7"/>
       <c r="F285" s="7"/>
       <c r="G285" s="0"/>
     </row>
-    <row r="286" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="14" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B286" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C286" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D286" s="13" t="n">
-        <v>-4</v>
+        <v>239</v>
+      </c>
+      <c r="D286" s="7" t="n">
+        <v>-2</v>
       </c>
       <c r="E286" s="7"/>
       <c r="F286" s="7"/>
@@ -7018,9 +6822,9 @@
       <c r="F287" s="0"/>
       <c r="G287" s="0"/>
     </row>
-    <row r="288" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="14" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B288" s="7" t="s">
         <v>231</v>
@@ -7043,60 +6847,62 @@
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B289" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C289" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D289" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="E289" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F289" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G289" s="12" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B290" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C290" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D290" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="E290" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F290" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G290" s="12" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B291" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C291" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D291" s="13" t="s">
         <v>278</v>
-      </c>
-      <c r="B289" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C289" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D289" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="E289" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F289" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G289" s="0"/>
-    </row>
-    <row r="290" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="B290" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C290" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D290" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="E290" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F290" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G290" s="19" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="291" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="B291" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C291" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D291" s="13" t="s">
-        <v>282</v>
       </c>
       <c r="E291" s="7"/>
       <c r="F291" s="7"/>
@@ -7104,23 +6910,23 @@
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="14" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B292" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C292" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D292" s="11" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="E292" s="7"/>
       <c r="F292" s="7"/>
       <c r="G292" s="0"/>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="0"/>
+      <c r="A293" s="14"/>
       <c r="B293" s="0"/>
       <c r="C293" s="0"/>
       <c r="D293" s="15"/>
@@ -7128,9 +6934,9 @@
       <c r="F293" s="0"/>
       <c r="G293" s="0"/>
     </row>
-    <row r="294" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="14" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B294" s="7" t="s">
         <v>231</v>
@@ -7153,7 +6959,7 @@
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="14" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B295" s="7" t="s">
         <v>231</v>
@@ -7161,20 +6967,22 @@
       <c r="C295" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D295" s="7" t="s">
-        <v>285</v>
+      <c r="D295" s="11" t="s">
+        <v>280</v>
       </c>
       <c r="E295" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F295" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G295" s="0"/>
+        <v>90</v>
+      </c>
+      <c r="G295" s="12" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="14" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B296" s="7" t="s">
         <v>231</v>
@@ -7182,31 +6990,31 @@
       <c r="C296" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D296" s="7" t="s">
-        <v>286</v>
+      <c r="D296" s="11" t="s">
+        <v>282</v>
       </c>
       <c r="E296" s="7" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F296" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G296" s="19" t="s">
-        <v>287</v>
+        <v>92</v>
+      </c>
+      <c r="G296" s="12" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="B297" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C297" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D297" s="13" t="s">
         <v>284</v>
-      </c>
-      <c r="B297" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C297" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D297" s="12" t="s">
-        <v>288</v>
       </c>
       <c r="E297" s="7"/>
       <c r="F297" s="7"/>
@@ -7214,16 +7022,16 @@
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="14" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B298" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C298" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D298" s="11" t="s">
-        <v>289</v>
+        <v>239</v>
+      </c>
+      <c r="D298" s="13" t="n">
+        <v>-3</v>
       </c>
       <c r="E298" s="7"/>
       <c r="F298" s="7"/>
@@ -7238,9 +7046,9 @@
       <c r="F299" s="0"/>
       <c r="G299" s="0"/>
     </row>
-    <row r="300" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="14" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B300" s="7" t="s">
         <v>231</v>
@@ -7263,7 +7071,7 @@
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="14" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B301" s="7" t="s">
         <v>231</v>
@@ -7272,7 +7080,7 @@
         <v>11</v>
       </c>
       <c r="D301" s="7" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E301" s="7" t="s">
         <v>33</v>
@@ -7284,7 +7092,7 @@
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="14" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B302" s="7" t="s">
         <v>231</v>
@@ -7293,7 +7101,7 @@
         <v>11</v>
       </c>
       <c r="D302" s="7" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E302" s="7" t="s">
         <v>22</v>
@@ -7301,22 +7109,22 @@
       <c r="F302" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G302" s="19" t="s">
-        <v>293</v>
+      <c r="G302" s="22" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="14" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B303" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C303" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D303" s="12" t="s">
-        <v>294</v>
+        <v>237</v>
+      </c>
+      <c r="D303" s="13" t="s">
+        <v>289</v>
       </c>
       <c r="E303" s="7"/>
       <c r="F303" s="7"/>
@@ -7324,16 +7132,16 @@
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="14" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B304" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C304" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D304" s="11" t="s">
-        <v>295</v>
+        <v>239</v>
+      </c>
+      <c r="D304" s="13" t="n">
+        <v>-4</v>
       </c>
       <c r="E304" s="7"/>
       <c r="F304" s="7"/>
@@ -7348,9 +7156,9 @@
       <c r="F305" s="0"/>
       <c r="G305" s="0"/>
     </row>
-    <row r="306" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="14" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B306" s="7" t="s">
         <v>231</v>
@@ -7371,9 +7179,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="307" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="14" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B307" s="7" t="s">
         <v>231</v>
@@ -7381,54 +7189,52 @@
       <c r="C307" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D307" s="11" t="s">
-        <v>297</v>
+      <c r="D307" s="7" t="s">
+        <v>291</v>
       </c>
       <c r="E307" s="7" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F307" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G307" s="0"/>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B308" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C308" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D308" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E308" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F308" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G307" s="12" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="308" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="B308" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C308" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D308" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="E308" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F308" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G308" s="12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="309" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G308" s="22" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="14" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B309" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C309" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D309" s="13" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E309" s="7"/>
       <c r="F309" s="7"/>
@@ -7436,13 +7242,13 @@
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="14" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B310" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C310" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D310" s="11" t="s">
         <v>295</v>
@@ -7460,9 +7266,9 @@
       <c r="F311" s="0"/>
       <c r="G311" s="0"/>
     </row>
-    <row r="312" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="14" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B312" s="7" t="s">
         <v>231</v>
@@ -7483,9 +7289,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="313" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="14" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B313" s="7" t="s">
         <v>231</v>
@@ -7493,71 +7299,69 @@
       <c r="C313" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D313" s="11" t="s">
-        <v>303</v>
+      <c r="D313" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="E313" s="7" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F313" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G313" s="0"/>
+    </row>
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="B314" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C314" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D314" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="E314" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F314" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G313" s="12" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="314" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="B314" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C314" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D314" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="E314" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F314" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G314" s="12" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="315" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G314" s="22" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="14" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B315" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C315" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D315" s="13" t="s">
-        <v>307</v>
+        <v>237</v>
+      </c>
+      <c r="D315" s="12" t="s">
+        <v>300</v>
       </c>
       <c r="E315" s="7"/>
       <c r="F315" s="7"/>
       <c r="G315" s="0"/>
     </row>
-    <row r="316" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="14" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B316" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C316" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D316" s="13" t="n">
-        <v>-3</v>
+        <v>239</v>
+      </c>
+      <c r="D316" s="11" t="s">
+        <v>301</v>
       </c>
       <c r="E316" s="7"/>
       <c r="F316" s="7"/>
@@ -7572,9 +7376,9 @@
       <c r="F317" s="0"/>
       <c r="G317" s="0"/>
     </row>
-    <row r="318" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="14" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B318" s="7" t="s">
         <v>231</v>
@@ -7595,9 +7399,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="319" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="14" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B319" s="7" t="s">
         <v>231</v>
@@ -7605,54 +7409,52 @@
       <c r="C319" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D319" s="11" t="s">
-        <v>309</v>
+      <c r="D319" s="7" t="s">
+        <v>303</v>
       </c>
       <c r="E319" s="7" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F319" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G319" s="0"/>
+    </row>
+    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="B320" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C320" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D320" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="E320" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F320" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G319" s="12" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="320" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="B320" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C320" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D320" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="E320" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F320" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G320" s="12" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="321" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G320" s="22" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="14" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B321" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C321" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D321" s="13" t="s">
-        <v>312</v>
+        <v>237</v>
+      </c>
+      <c r="D321" s="12" t="s">
+        <v>306</v>
       </c>
       <c r="E321" s="7"/>
       <c r="F321" s="7"/>
@@ -7660,16 +7462,16 @@
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="14" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B322" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C322" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D322" s="11" t="s">
-        <v>241</v>
+        <v>307</v>
       </c>
       <c r="E322" s="7"/>
       <c r="F322" s="7"/>
@@ -7684,9 +7486,9 @@
       <c r="F323" s="0"/>
       <c r="G323" s="0"/>
     </row>
-    <row r="324" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="14" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B324" s="7" t="s">
         <v>231</v>
@@ -7707,9 +7509,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="325" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="14" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B325" s="7" t="s">
         <v>231</v>
@@ -7718,7 +7520,7 @@
         <v>11</v>
       </c>
       <c r="D325" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E325" s="7" t="s">
         <v>22</v>
@@ -7727,12 +7529,12 @@
         <v>90</v>
       </c>
       <c r="G325" s="12" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="326" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="14" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B326" s="7" t="s">
         <v>231</v>
@@ -7741,30 +7543,30 @@
         <v>11</v>
       </c>
       <c r="D326" s="11" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E326" s="7" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F326" s="7" t="s">
         <v>92</v>
       </c>
       <c r="G326" s="12" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="327" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B327" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C327" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D327" s="13" t="s">
         <v>313</v>
-      </c>
-      <c r="B327" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C327" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D327" s="13" t="s">
-        <v>318</v>
       </c>
       <c r="E327" s="7"/>
       <c r="F327" s="7"/>
@@ -7772,33 +7574,33 @@
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="14" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B328" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C328" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D328" s="11" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="E328" s="7"/>
       <c r="F328" s="7"/>
       <c r="G328" s="0"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="14"/>
-      <c r="B329" s="7"/>
-      <c r="C329" s="7"/>
-      <c r="D329" s="11"/>
-      <c r="E329" s="7"/>
-      <c r="F329" s="7"/>
+      <c r="A329" s="0"/>
+      <c r="B329" s="0"/>
+      <c r="C329" s="0"/>
+      <c r="D329" s="15"/>
+      <c r="E329" s="0"/>
+      <c r="F329" s="0"/>
       <c r="G329" s="0"/>
     </row>
-    <row r="330" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B330" s="7" t="s">
         <v>231</v>
@@ -7819,9 +7621,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B331" s="7" t="s">
         <v>231</v>
@@ -7830,7 +7632,7 @@
         <v>11</v>
       </c>
       <c r="D331" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E331" s="7" t="s">
         <v>22</v>
@@ -7839,12 +7641,12 @@
         <v>90</v>
       </c>
       <c r="G331" s="12" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="332" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B332" s="7" t="s">
         <v>231</v>
@@ -7853,30 +7655,30 @@
         <v>11</v>
       </c>
       <c r="D332" s="11" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E332" s="7" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F332" s="7" t="s">
         <v>92</v>
       </c>
       <c r="G332" s="12" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="333" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B333" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C333" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D333" s="13" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="E333" s="7"/>
       <c r="F333" s="7"/>
@@ -7884,33 +7686,33 @@
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B334" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C334" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D334" s="11" t="s">
-        <v>241</v>
+        <v>239</v>
+      </c>
+      <c r="D334" s="13" t="n">
+        <v>-3</v>
       </c>
       <c r="E334" s="7"/>
       <c r="F334" s="7"/>
       <c r="G334" s="0"/>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A335" s="14"/>
-      <c r="B335" s="7"/>
-      <c r="C335" s="7"/>
-      <c r="D335" s="11"/>
-      <c r="E335" s="7"/>
-      <c r="F335" s="7"/>
+      <c r="A335" s="0"/>
+      <c r="B335" s="0"/>
+      <c r="C335" s="0"/>
+      <c r="D335" s="15"/>
+      <c r="E335" s="0"/>
+      <c r="F335" s="0"/>
       <c r="G335" s="0"/>
     </row>
-    <row r="336" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="14" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B336" s="7" t="s">
         <v>231</v>
@@ -7931,9 +7733,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="14" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B337" s="7" t="s">
         <v>231</v>
@@ -7942,7 +7744,7 @@
         <v>11</v>
       </c>
       <c r="D337" s="11" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E337" s="7" t="s">
         <v>22</v>
@@ -7951,12 +7753,12 @@
         <v>90</v>
       </c>
       <c r="G337" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="338" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="14" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B338" s="7" t="s">
         <v>231</v>
@@ -7965,7 +7767,7 @@
         <v>11</v>
       </c>
       <c r="D338" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="E338" s="7" t="s">
         <v>22</v>
@@ -7974,21 +7776,21 @@
         <v>92</v>
       </c>
       <c r="G338" s="12" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="339" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="14" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B339" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C339" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D339" s="13" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="E339" s="7"/>
       <c r="F339" s="7"/>
@@ -7996,16 +7798,16 @@
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="14" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B340" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C340" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D340" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="D340" s="11" t="s">
-        <v>241</v>
       </c>
       <c r="E340" s="7"/>
       <c r="F340" s="7"/>
@@ -8022,7 +7824,7 @@
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="14" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B342" s="7" t="s">
         <v>231</v>
@@ -8045,7 +7847,7 @@
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="14" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B343" s="7" t="s">
         <v>231</v>
@@ -8054,21 +7856,21 @@
         <v>11</v>
       </c>
       <c r="D343" s="11" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="E343" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F343" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G343" s="12" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="14" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B344" s="7" t="s">
         <v>231</v>
@@ -8077,64 +7879,64 @@
         <v>11</v>
       </c>
       <c r="D344" s="11" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="E344" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F344" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G344" s="12" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="14" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B345" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C345" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D345" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="E345" s="0"/>
+        <v>237</v>
+      </c>
+      <c r="D345" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="E345" s="7"/>
       <c r="F345" s="7"/>
       <c r="G345" s="0"/>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="B346" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C346" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D346" s="11" t="s">
         <v>331</v>
-      </c>
-      <c r="B346" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C346" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D346" s="11" t="s">
-        <v>295</v>
       </c>
       <c r="E346" s="7"/>
       <c r="F346" s="7"/>
       <c r="G346" s="0"/>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A347" s="0"/>
-      <c r="B347" s="0"/>
-      <c r="C347" s="0"/>
-      <c r="D347" s="15"/>
-      <c r="E347" s="0"/>
-      <c r="F347" s="0"/>
+      <c r="A347" s="14"/>
+      <c r="B347" s="7"/>
+      <c r="C347" s="7"/>
+      <c r="D347" s="11"/>
+      <c r="E347" s="7"/>
+      <c r="F347" s="7"/>
       <c r="G347" s="0"/>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="14" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B348" s="7" t="s">
         <v>231</v>
@@ -8157,7 +7959,7 @@
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="14" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B349" s="7" t="s">
         <v>231</v>
@@ -8166,21 +7968,21 @@
         <v>11</v>
       </c>
       <c r="D349" s="11" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="E349" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F349" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G349" s="12" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="14" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B350" s="7" t="s">
         <v>231</v>
@@ -8189,30 +7991,30 @@
         <v>11</v>
       </c>
       <c r="D350" s="11" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="E350" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F350" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G350" s="12" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="B351" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C351" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D351" s="13" t="s">
         <v>337</v>
-      </c>
-      <c r="B351" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C351" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D351" s="13" t="s">
-        <v>342</v>
       </c>
       <c r="E351" s="7"/>
       <c r="F351" s="7"/>
@@ -8220,33 +8022,33 @@
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="14" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B352" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C352" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D352" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="D352" s="11" t="s">
-        <v>295</v>
       </c>
       <c r="E352" s="7"/>
       <c r="F352" s="7"/>
       <c r="G352" s="0"/>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="0"/>
-      <c r="B353" s="0"/>
-      <c r="C353" s="0"/>
-      <c r="D353" s="15"/>
-      <c r="E353" s="0"/>
-      <c r="F353" s="0"/>
+      <c r="A353" s="14"/>
+      <c r="B353" s="7"/>
+      <c r="C353" s="7"/>
+      <c r="D353" s="11"/>
+      <c r="E353" s="7"/>
+      <c r="F353" s="7"/>
       <c r="G353" s="0"/>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="14" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B354" s="7" t="s">
         <v>231</v>
@@ -8269,7 +8071,7 @@
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="14" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B355" s="7" t="s">
         <v>231</v>
@@ -8277,20 +8079,22 @@
       <c r="C355" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D355" s="7" t="s">
-        <v>344</v>
+      <c r="D355" s="11" t="s">
+        <v>339</v>
       </c>
       <c r="E355" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F355" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G355" s="0"/>
+        <v>90</v>
+      </c>
+      <c r="G355" s="12" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="14" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B356" s="7" t="s">
         <v>231</v>
@@ -8298,29 +8102,31 @@
       <c r="C356" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D356" s="7" t="s">
-        <v>345</v>
+      <c r="D356" s="11" t="s">
+        <v>341</v>
       </c>
       <c r="E356" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F356" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G356" s="0"/>
+        <v>92</v>
+      </c>
+      <c r="G356" s="12" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="14" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B357" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C357" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D357" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
+      </c>
+      <c r="D357" s="13" t="s">
+        <v>342</v>
       </c>
       <c r="E357" s="7"/>
       <c r="F357" s="7"/>
@@ -8328,16 +8134,16 @@
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="14" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B358" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C358" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D358" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="D358" s="11" t="s">
-        <v>241</v>
       </c>
       <c r="E358" s="7"/>
       <c r="F358" s="7"/>
@@ -8353,1799 +8159,46 @@
       <c r="G359" s="0"/>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="14" t="s">
+      <c r="A360" s="0"/>
+      <c r="B360" s="0"/>
+      <c r="C360" s="0"/>
+      <c r="D360" s="15"/>
+      <c r="E360" s="0"/>
+      <c r="F360" s="0"/>
+      <c r="G360" s="0"/>
+    </row>
+    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B361" s="9"/>
+      <c r="C361" s="9"/>
+      <c r="D361" s="10"/>
+      <c r="E361" s="9"/>
+      <c r="F361" s="9"/>
+      <c r="G361" s="9"/>
+    </row>
+    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="B362" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="C362" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D362" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="B360" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C360" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D360" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E360" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F360" s="7" t="s">
+      <c r="E362" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F362" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G360" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="B361" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C361" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D361" s="11" t="s">
+      <c r="G362" s="12" t="s">
         <v>347</v>
-      </c>
-      <c r="E361" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F361" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G361" s="12" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="B362" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C362" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D362" s="11" t="s">
-        <v>349</v>
-      </c>
-      <c r="E362" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F362" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G362" s="12" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A363" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="B363" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C363" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D363" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="E363" s="7"/>
-      <c r="F363" s="7"/>
-      <c r="G363" s="0"/>
-    </row>
-    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A364" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="B364" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C364" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D364" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="E364" s="7"/>
-      <c r="F364" s="7"/>
-      <c r="G364" s="0"/>
-    </row>
-    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A365" s="0"/>
-      <c r="B365" s="0"/>
-      <c r="C365" s="0"/>
-      <c r="D365" s="15"/>
-      <c r="E365" s="0"/>
-      <c r="F365" s="0"/>
-      <c r="G365" s="0"/>
-    </row>
-    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A366" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="B366" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C366" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D366" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E366" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F366" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G366" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A367" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="B367" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C367" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D367" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="E367" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F367" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G367" s="0"/>
-    </row>
-    <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A368" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="B368" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C368" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D368" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="E368" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F368" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G368" s="19" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A369" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="B369" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C369" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D369" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="E369" s="7"/>
-      <c r="F369" s="7"/>
-      <c r="G369" s="0"/>
-    </row>
-    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A370" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="B370" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C370" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D370" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="E370" s="7"/>
-      <c r="F370" s="7"/>
-      <c r="G370" s="0"/>
-    </row>
-    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A371" s="0"/>
-      <c r="B371" s="0"/>
-      <c r="C371" s="0"/>
-      <c r="D371" s="15"/>
-      <c r="E371" s="0"/>
-      <c r="F371" s="0"/>
-      <c r="G371" s="0"/>
-    </row>
-    <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A372" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="B372" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C372" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D372" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E372" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F372" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G372" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A373" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="B373" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C373" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D373" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="E373" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F373" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G373" s="0"/>
-    </row>
-    <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A374" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="B374" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C374" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D374" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="E374" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F374" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G374" s="19" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A375" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="B375" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C375" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D375" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="E375" s="7"/>
-      <c r="F375" s="7"/>
-      <c r="G375" s="0"/>
-    </row>
-    <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A376" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="B376" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C376" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D376" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="E376" s="7"/>
-      <c r="F376" s="7"/>
-      <c r="G376" s="0"/>
-    </row>
-    <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A377" s="0"/>
-      <c r="B377" s="0"/>
-      <c r="C377" s="0"/>
-      <c r="D377" s="15"/>
-      <c r="E377" s="0"/>
-      <c r="F377" s="0"/>
-      <c r="G377" s="0"/>
-    </row>
-    <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A378" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="B378" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C378" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D378" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E378" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F378" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G378" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A379" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="B379" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C379" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D379" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="E379" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F379" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G379" s="0"/>
-    </row>
-    <row r="380" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A380" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="B380" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C380" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D380" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="E380" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F380" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G380" s="19" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A381" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="B381" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C381" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D381" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="E381" s="7"/>
-      <c r="F381" s="7"/>
-      <c r="G381" s="0"/>
-    </row>
-    <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A382" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="B382" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C382" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D382" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="E382" s="7"/>
-      <c r="F382" s="7"/>
-      <c r="G382" s="0"/>
-    </row>
-    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A383" s="0"/>
-      <c r="B383" s="0"/>
-      <c r="C383" s="0"/>
-      <c r="D383" s="15"/>
-      <c r="E383" s="0"/>
-      <c r="F383" s="0"/>
-      <c r="G383" s="0"/>
-    </row>
-    <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A384" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="B384" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C384" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D384" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E384" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F384" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G384" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A385" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="B385" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C385" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D385" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="E385" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F385" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G385" s="0"/>
-    </row>
-    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A386" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="B386" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C386" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D386" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="E386" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F386" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G386" s="19" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A387" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="B387" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C387" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D387" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="E387" s="7"/>
-      <c r="F387" s="7"/>
-      <c r="G387" s="0"/>
-    </row>
-    <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A388" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="B388" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C388" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D388" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="E388" s="7"/>
-      <c r="F388" s="7"/>
-      <c r="G388" s="0"/>
-    </row>
-    <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="0"/>
-      <c r="B389" s="0"/>
-      <c r="C389" s="0"/>
-      <c r="D389" s="15"/>
-      <c r="E389" s="0"/>
-      <c r="F389" s="0"/>
-      <c r="G389" s="0"/>
-    </row>
-    <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A390" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="B390" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C390" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D390" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E390" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F390" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G390" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="B391" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C391" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D391" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="E391" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F391" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G391" s="0"/>
-    </row>
-    <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A392" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="B392" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C392" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D392" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="E392" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F392" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G392" s="19" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A393" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="B393" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C393" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D393" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="E393" s="7"/>
-      <c r="F393" s="7"/>
-      <c r="G393" s="0"/>
-    </row>
-    <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A394" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="B394" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C394" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D394" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="E394" s="7"/>
-      <c r="F394" s="7"/>
-      <c r="G394" s="0"/>
-    </row>
-    <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A395" s="0"/>
-      <c r="B395" s="0"/>
-      <c r="C395" s="0"/>
-      <c r="D395" s="15"/>
-      <c r="E395" s="0"/>
-      <c r="F395" s="0"/>
-      <c r="G395" s="0"/>
-    </row>
-    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A396" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="B396" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C396" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D396" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E396" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F396" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G396" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A397" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="B397" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C397" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D397" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="E397" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F397" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G397" s="0"/>
-    </row>
-    <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A398" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="B398" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C398" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D398" s="7" t="s">
-        <v>375</v>
-      </c>
-      <c r="E398" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F398" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G398" s="19" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A399" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="B399" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C399" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D399" s="12" t="s">
-        <v>377</v>
-      </c>
-      <c r="E399" s="7"/>
-      <c r="F399" s="7"/>
-      <c r="G399" s="0"/>
-    </row>
-    <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A400" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="B400" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C400" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D400" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="E400" s="7"/>
-      <c r="F400" s="7"/>
-      <c r="G400" s="0"/>
-    </row>
-    <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A401" s="0"/>
-      <c r="B401" s="0"/>
-      <c r="C401" s="0"/>
-      <c r="D401" s="15"/>
-      <c r="E401" s="0"/>
-      <c r="F401" s="0"/>
-      <c r="G401" s="0"/>
-    </row>
-    <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A402" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="B402" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C402" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D402" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E402" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F402" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G402" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A403" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="B403" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C403" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D403" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="E403" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F403" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G403" s="0"/>
-    </row>
-    <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A404" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="B404" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C404" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D404" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="E404" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F404" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G404" s="19" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="B405" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C405" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D405" s="12" t="s">
-        <v>382</v>
-      </c>
-      <c r="E405" s="7"/>
-      <c r="F405" s="7"/>
-      <c r="G405" s="0"/>
-    </row>
-    <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A406" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="B406" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C406" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D406" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="E406" s="7"/>
-      <c r="F406" s="7"/>
-      <c r="G406" s="0"/>
-    </row>
-    <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A407" s="0"/>
-      <c r="B407" s="0"/>
-      <c r="C407" s="0"/>
-      <c r="D407" s="15"/>
-      <c r="E407" s="0"/>
-      <c r="F407" s="0"/>
-      <c r="G407" s="0"/>
-    </row>
-    <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A408" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="B408" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C408" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D408" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E408" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F408" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G408" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A409" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="B409" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C409" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D409" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="E409" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F409" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G409" s="0"/>
-    </row>
-    <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="B410" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C410" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D410" s="7" t="s">
-        <v>385</v>
-      </c>
-      <c r="E410" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F410" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G410" s="19" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A411" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="B411" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C411" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D411" s="12" t="s">
-        <v>382</v>
-      </c>
-      <c r="E411" s="7"/>
-      <c r="F411" s="7"/>
-      <c r="G411" s="0"/>
-    </row>
-    <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A412" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="B412" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C412" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D412" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="E412" s="7"/>
-      <c r="F412" s="7"/>
-      <c r="G412" s="0"/>
-    </row>
-    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A413" s="0"/>
-      <c r="B413" s="0"/>
-      <c r="C413" s="0"/>
-      <c r="D413" s="15"/>
-      <c r="E413" s="0"/>
-      <c r="F413" s="0"/>
-      <c r="G413" s="0"/>
-    </row>
-    <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A414" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="B414" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C414" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D414" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E414" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F414" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G414" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A415" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="B415" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C415" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D415" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="E415" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F415" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G415" s="0"/>
-    </row>
-    <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A416" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="B416" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C416" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D416" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="E416" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F416" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G416" s="19" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A417" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="B417" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C417" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D417" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="E417" s="7"/>
-      <c r="F417" s="7"/>
-      <c r="G417" s="0"/>
-    </row>
-    <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A418" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="B418" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C418" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D418" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="E418" s="7"/>
-      <c r="F418" s="7"/>
-      <c r="G418" s="0"/>
-    </row>
-    <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A419" s="0"/>
-      <c r="B419" s="0"/>
-      <c r="C419" s="0"/>
-      <c r="D419" s="15"/>
-      <c r="E419" s="0"/>
-      <c r="F419" s="0"/>
-      <c r="G419" s="0"/>
-    </row>
-    <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A420" s="14" t="s">
-        <v>392</v>
-      </c>
-      <c r="B420" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C420" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D420" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E420" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F420" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G420" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A421" s="14" t="s">
-        <v>392</v>
-      </c>
-      <c r="B421" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C421" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D421" s="7" t="s">
-        <v>393</v>
-      </c>
-      <c r="E421" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F421" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G421" s="0"/>
-    </row>
-    <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A422" s="14" t="s">
-        <v>392</v>
-      </c>
-      <c r="B422" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C422" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D422" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="E422" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F422" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G422" s="0" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="14" t="s">
-        <v>392</v>
-      </c>
-      <c r="B423" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C423" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D423" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="E423" s="7"/>
-      <c r="F423" s="7"/>
-      <c r="G423" s="0"/>
-    </row>
-    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A424" s="14" t="s">
-        <v>392</v>
-      </c>
-      <c r="B424" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C424" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D424" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="E424" s="7"/>
-      <c r="F424" s="7"/>
-      <c r="G424" s="0"/>
-    </row>
-    <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A425" s="0"/>
-      <c r="B425" s="0"/>
-      <c r="C425" s="0"/>
-      <c r="D425" s="15"/>
-      <c r="E425" s="0"/>
-      <c r="F425" s="0"/>
-      <c r="G425" s="0"/>
-    </row>
-    <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A426" s="14" t="s">
-        <v>397</v>
-      </c>
-      <c r="B426" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C426" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D426" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E426" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F426" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G426" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A427" s="14" t="s">
-        <v>397</v>
-      </c>
-      <c r="B427" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C427" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D427" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="E427" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F427" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G427" s="0"/>
-    </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A428" s="14" t="s">
-        <v>397</v>
-      </c>
-      <c r="B428" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C428" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D428" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="E428" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F428" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G428" s="19" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A429" s="14" t="s">
-        <v>397</v>
-      </c>
-      <c r="B429" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C429" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D429" s="12" t="s">
-        <v>401</v>
-      </c>
-      <c r="E429" s="7"/>
-      <c r="F429" s="7"/>
-      <c r="G429" s="0"/>
-    </row>
-    <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A430" s="14" t="s">
-        <v>397</v>
-      </c>
-      <c r="B430" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C430" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D430" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="E430" s="7"/>
-      <c r="F430" s="7"/>
-      <c r="G430" s="0"/>
-    </row>
-    <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="0"/>
-      <c r="B431" s="0"/>
-      <c r="C431" s="0"/>
-      <c r="D431" s="15"/>
-      <c r="E431" s="0"/>
-      <c r="F431" s="0"/>
-      <c r="G431" s="0"/>
-    </row>
-    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="14" t="s">
-        <v>402</v>
-      </c>
-      <c r="B432" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C432" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D432" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E432" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F432" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G432" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="14" t="s">
-        <v>402</v>
-      </c>
-      <c r="B433" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C433" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D433" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="E433" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F433" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G433" s="0"/>
-    </row>
-    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="14" t="s">
-        <v>402</v>
-      </c>
-      <c r="B434" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C434" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D434" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="E434" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F434" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G434" s="19" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="14" t="s">
-        <v>402</v>
-      </c>
-      <c r="B435" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C435" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D435" s="12" t="s">
-        <v>406</v>
-      </c>
-      <c r="E435" s="0"/>
-      <c r="F435" s="7"/>
-      <c r="G435" s="0"/>
-    </row>
-    <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="14" t="s">
-        <v>402</v>
-      </c>
-      <c r="B436" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C436" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D436" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="E436" s="7"/>
-      <c r="F436" s="7"/>
-      <c r="G436" s="0"/>
-    </row>
-    <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A437" s="14"/>
-      <c r="B437" s="7"/>
-      <c r="C437" s="7"/>
-      <c r="D437" s="11"/>
-      <c r="E437" s="7"/>
-      <c r="F437" s="7"/>
-      <c r="G437" s="0"/>
-    </row>
-    <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A438" s="14" t="s">
-        <v>407</v>
-      </c>
-      <c r="B438" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C438" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D438" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E438" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F438" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G438" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A439" s="14" t="s">
-        <v>407</v>
-      </c>
-      <c r="B439" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C439" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D439" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="E439" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F439" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G439" s="0"/>
-    </row>
-    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A440" s="14" t="s">
-        <v>407</v>
-      </c>
-      <c r="B440" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C440" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D440" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="E440" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F440" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G440" s="19" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="14" t="s">
-        <v>407</v>
-      </c>
-      <c r="B441" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C441" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D441" s="12" t="s">
-        <v>411</v>
-      </c>
-      <c r="E441" s="0"/>
-      <c r="F441" s="7"/>
-      <c r="G441" s="0"/>
-    </row>
-    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A442" s="14" t="s">
-        <v>407</v>
-      </c>
-      <c r="B442" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C442" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D442" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="E442" s="7"/>
-      <c r="F442" s="7"/>
-      <c r="G442" s="0"/>
-    </row>
-    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="0"/>
-      <c r="B443" s="0"/>
-      <c r="C443" s="0"/>
-      <c r="D443" s="15"/>
-      <c r="E443" s="0"/>
-      <c r="F443" s="0"/>
-      <c r="G443" s="0"/>
-    </row>
-    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A444" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="B444" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C444" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D444" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E444" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F444" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G444" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A445" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="B445" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C445" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D445" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="E445" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F445" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G445" s="0"/>
-    </row>
-    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A446" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="B446" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C446" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D446" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="E446" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F446" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G446" s="19" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A447" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="B447" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C447" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D447" s="12" t="s">
-        <v>416</v>
-      </c>
-      <c r="E447" s="0"/>
-      <c r="F447" s="7"/>
-      <c r="G447" s="0"/>
-    </row>
-    <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A448" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="B448" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C448" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D448" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="E448" s="7"/>
-      <c r="F448" s="7"/>
-      <c r="G448" s="0"/>
-    </row>
-    <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="0"/>
-      <c r="B449" s="0"/>
-      <c r="C449" s="0"/>
-      <c r="D449" s="15"/>
-      <c r="E449" s="0"/>
-      <c r="F449" s="0"/>
-      <c r="G449" s="0"/>
-    </row>
-    <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A450" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="B450" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C450" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D450" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E450" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F450" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G450" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A451" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="B451" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C451" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D451" s="7" t="s">
-        <v>418</v>
-      </c>
-      <c r="E451" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F451" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G451" s="0"/>
-    </row>
-    <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A452" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="B452" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C452" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D452" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="E452" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F452" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G452" s="19" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A453" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="B453" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C453" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D453" s="12" t="s">
-        <v>421</v>
-      </c>
-      <c r="E453" s="0"/>
-      <c r="F453" s="7"/>
-      <c r="G453" s="0"/>
-    </row>
-    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A454" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="B454" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C454" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D454" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="E454" s="7"/>
-      <c r="F454" s="7"/>
-      <c r="G454" s="0"/>
-    </row>
-    <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A455" s="0"/>
-      <c r="B455" s="0"/>
-      <c r="C455" s="0"/>
-      <c r="D455" s="15"/>
-      <c r="E455" s="0"/>
-      <c r="F455" s="0"/>
-      <c r="G455" s="0"/>
-    </row>
-    <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A456" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="B456" s="9"/>
-      <c r="C456" s="9"/>
-      <c r="D456" s="10"/>
-      <c r="E456" s="9"/>
-      <c r="F456" s="9"/>
-      <c r="G456" s="9"/>
-    </row>
-    <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A457" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="B457" s="7" t="s">
-        <v>424</v>
-      </c>
-      <c r="C457" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D457" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="E457" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F457" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G457" s="12" t="s">
-        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>